<commit_message>
Supplemental cost curve calcs for sensitivity analysis
</commit_message>
<xml_diff>
--- a/Studies/co_analysis/Agrivoltaics Row Spacing Cost Curve.xlsx
+++ b/Studies/co_analysis/Agrivoltaics Row Spacing Cost Curve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmirletz\source\repos\agrivoltaics\co_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmirletz\source\repos\InSPIRE\Studies\co_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5C5EC3-206A-47BF-A4AC-45FAF5B280DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9FB1A4-5531-48E9-B5F2-44925F8CF965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1308" yWindow="924" windowWidth="21600" windowHeight="11232" xr2:uid="{B53101FC-5DD3-4F15-A582-1FB9B136D146}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B53101FC-5DD3-4F15-A582-1FB9B136D146}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -142,11 +142,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +485,7 @@
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,47 +575,47 @@
         <v>1.3004497785262972</v>
       </c>
       <c r="H2" s="1">
-        <f>$G$2+H$16*($D$2-$D2)</f>
+        <f t="shared" ref="H2:R14" si="1">$G$2+H$16*($D$2-$D2)</f>
         <v>1.3004497785262972</v>
       </c>
       <c r="I2" s="1">
-        <f>$G$2+I$16*($D$2-$D2)</f>
+        <f t="shared" si="1"/>
         <v>1.3004497785262972</v>
       </c>
       <c r="J2" s="1">
-        <f>$G$2+J$16*($D$2-$D2)</f>
+        <f t="shared" si="1"/>
         <v>1.3004497785262972</v>
       </c>
       <c r="K2" s="1">
-        <f>$G$2+K$16*($D$2-$D2)</f>
+        <f t="shared" si="1"/>
         <v>1.3004497785262972</v>
       </c>
       <c r="L2" s="1">
-        <f>$G$2+L$16*($D$2-$D2)</f>
+        <f t="shared" si="1"/>
         <v>1.3004497785262972</v>
       </c>
       <c r="M2" s="1">
-        <f>$G$2+M$16*($D$2-$D2)</f>
+        <f t="shared" si="1"/>
         <v>1.3004497785262972</v>
       </c>
       <c r="N2" s="1">
-        <f>$G$2+N$16*($D$2-$D2)</f>
+        <f t="shared" si="1"/>
         <v>1.3004497785262972</v>
       </c>
       <c r="O2" s="1">
-        <f>$G$2+O$16*($D$2-$D2)</f>
+        <f t="shared" si="1"/>
         <v>1.3004497785262972</v>
       </c>
       <c r="P2" s="1">
-        <f>$G$2+P$16*($D$2-$D2)</f>
+        <f t="shared" si="1"/>
         <v>1.3004497785262972</v>
       </c>
       <c r="Q2" s="1">
-        <f>$G$2+Q$16*($D$2-$D2)</f>
+        <f t="shared" si="1"/>
         <v>1.3004497785262972</v>
       </c>
       <c r="R2" s="1">
-        <f>$G$2+R$16*($D$2-$D2)</f>
+        <f t="shared" si="1"/>
         <v>1.3004497785262972</v>
       </c>
       <c r="S2" s="1"/>
@@ -645,7 +646,7 @@
         <v>21.7</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C14" si="1">B3*0.3048</f>
+        <f t="shared" ref="C3:C14" si="2">B3*0.3048</f>
         <v>6.61416</v>
       </c>
       <c r="D3">
@@ -662,51 +663,54 @@
         <v>1.3526972371068819</v>
       </c>
       <c r="H3" s="1">
-        <f>$G$2+H$16*($D$2-$D3)</f>
+        <f t="shared" si="1"/>
         <v>1.3524497785262972</v>
       </c>
       <c r="I3" s="1">
-        <f>$G$2+I$16*($D$2-$D3)</f>
+        <f t="shared" si="1"/>
         <v>1.3628497785262972</v>
       </c>
       <c r="J3" s="1">
-        <f>$G$2+J$16*($D$2-$D3)</f>
+        <f t="shared" si="1"/>
         <v>1.3732497785262971</v>
       </c>
       <c r="K3" s="1">
-        <f>$G$2+K$16*($D$2-$D3)</f>
+        <f t="shared" si="1"/>
         <v>1.3836497785262971</v>
       </c>
       <c r="L3" s="1">
-        <f>$G$2+L$16*($D$2-$D3)</f>
+        <f t="shared" si="1"/>
         <v>1.3940497785262973</v>
       </c>
       <c r="M3" s="1">
-        <f>$G$2+M$16*($D$2-$D3)</f>
+        <f t="shared" si="1"/>
         <v>1.4044497785262973</v>
       </c>
       <c r="N3" s="1">
-        <f>$G$2+N$16*($D$2-$D3)</f>
+        <f t="shared" si="1"/>
         <v>1.4148497785262972</v>
       </c>
       <c r="O3" s="1">
-        <f>$G$2+O$16*($D$2-$D3)</f>
+        <f t="shared" si="1"/>
         <v>1.4252497785262972</v>
       </c>
       <c r="P3" s="1">
-        <f>$G$2+P$16*($D$2-$D3)</f>
+        <f t="shared" si="1"/>
         <v>1.4356497785262972</v>
       </c>
       <c r="Q3" s="1">
-        <f>$G$2+Q$16*($D$2-$D3)</f>
+        <f t="shared" si="1"/>
         <v>1.4460497785262971</v>
       </c>
       <c r="R3" s="1">
-        <f>$G$2+R$16*($D$2-$D3)</f>
+        <f t="shared" si="1"/>
         <v>1.4564497785262973</v>
       </c>
       <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
+      <c r="T3" s="4">
+        <f>0.01/G3</f>
+        <v>7.3926372625612606E-3</v>
+      </c>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
@@ -733,7 +737,7 @@
         <v>26.7</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.1381600000000009</v>
       </c>
       <c r="D4">
@@ -750,47 +754,47 @@
         <v>1.3849528948676084</v>
       </c>
       <c r="H4" s="1">
-        <f>$G$2+H$16*($D$2-$D4)</f>
+        <f t="shared" si="1"/>
         <v>1.3849497785262972</v>
       </c>
       <c r="I4" s="1">
-        <f>$G$2+I$16*($D$2-$D4)</f>
+        <f t="shared" si="1"/>
         <v>1.4018497785262971</v>
       </c>
       <c r="J4" s="1">
-        <f>$G$2+J$16*($D$2-$D4)</f>
+        <f t="shared" si="1"/>
         <v>1.4187497785262972</v>
       </c>
       <c r="K4" s="1">
-        <f>$G$2+K$16*($D$2-$D4)</f>
+        <f t="shared" si="1"/>
         <v>1.4356497785262972</v>
       </c>
       <c r="L4" s="1">
-        <f>$G$2+L$16*($D$2-$D4)</f>
+        <f t="shared" si="1"/>
         <v>1.4525497785262971</v>
       </c>
       <c r="M4" s="1">
-        <f>$G$2+M$16*($D$2-$D4)</f>
+        <f t="shared" si="1"/>
         <v>1.4694497785262972</v>
       </c>
       <c r="N4" s="1">
-        <f>$G$2+N$16*($D$2-$D4)</f>
+        <f t="shared" si="1"/>
         <v>1.4863497785262971</v>
       </c>
       <c r="O4" s="1">
-        <f>$G$2+O$16*($D$2-$D4)</f>
+        <f t="shared" si="1"/>
         <v>1.503249778526297</v>
       </c>
       <c r="P4" s="1">
-        <f>$G$2+P$16*($D$2-$D4)</f>
+        <f t="shared" si="1"/>
         <v>1.5201497785262972</v>
       </c>
       <c r="Q4" s="1">
-        <f>$G$2+Q$16*($D$2-$D4)</f>
+        <f t="shared" si="1"/>
         <v>1.5370497785262971</v>
       </c>
       <c r="R4" s="1">
-        <f>$G$2+R$16*($D$2-$D4)</f>
+        <f t="shared" si="1"/>
         <v>1.5539497785262972</v>
       </c>
       <c r="S4" s="1"/>
@@ -821,7 +825,7 @@
         <v>31.7</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.6621600000000001</v>
       </c>
       <c r="D5">
@@ -838,51 +842,54 @@
         <v>1.4063551938309375</v>
       </c>
       <c r="H5" s="1">
-        <f>$G$2+H$16*($D$2-$D5)</f>
+        <f t="shared" si="1"/>
         <v>1.4069497785262972</v>
       </c>
       <c r="I5" s="1">
-        <f>$G$2+I$16*($D$2-$D5)</f>
+        <f t="shared" si="1"/>
         <v>1.4282497785262971</v>
       </c>
       <c r="J5" s="1">
-        <f>$G$2+J$16*($D$2-$D5)</f>
+        <f t="shared" si="1"/>
         <v>1.4495497785262972</v>
       </c>
       <c r="K5" s="1">
-        <f>$G$2+K$16*($D$2-$D5)</f>
+        <f t="shared" si="1"/>
         <v>1.4708497785262971</v>
       </c>
       <c r="L5" s="1">
-        <f>$G$2+L$16*($D$2-$D5)</f>
+        <f t="shared" si="1"/>
         <v>1.4921497785262972</v>
       </c>
       <c r="M5" s="1">
-        <f>$G$2+M$16*($D$2-$D5)</f>
+        <f t="shared" si="1"/>
         <v>1.5134497785262973</v>
       </c>
       <c r="N5" s="1">
-        <f>$G$2+N$16*($D$2-$D5)</f>
+        <f t="shared" si="1"/>
         <v>1.5347497785262971</v>
       </c>
       <c r="O5" s="1">
-        <f>$G$2+O$16*($D$2-$D5)</f>
+        <f t="shared" si="1"/>
         <v>1.5560497785262972</v>
       </c>
       <c r="P5" s="1">
-        <f>$G$2+P$16*($D$2-$D5)</f>
+        <f t="shared" si="1"/>
         <v>1.5773497785262971</v>
       </c>
       <c r="Q5" s="1">
-        <f>$G$2+Q$16*($D$2-$D5)</f>
+        <f t="shared" si="1"/>
         <v>1.5986497785262972</v>
       </c>
       <c r="R5" s="1">
-        <f>$G$2+R$16*($D$2-$D5)</f>
+        <f t="shared" si="1"/>
         <v>1.6199497785262973</v>
       </c>
       <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
+      <c r="T5" s="4">
+        <f>0.05/G5</f>
+        <v>3.5552896038872711E-2</v>
+      </c>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -910,7 +917,7 @@
         <v>36.700000000000003</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11.186160000000001</v>
       </c>
       <c r="D6">
@@ -927,47 +934,47 @@
         <v>1.4230888104453481</v>
       </c>
       <c r="H6" s="1">
-        <f>$G$2+H$16*($D$2-$D6)</f>
+        <f t="shared" si="1"/>
         <v>1.4229497785262972</v>
       </c>
       <c r="I6" s="1">
-        <f>$G$2+I$16*($D$2-$D6)</f>
+        <f t="shared" si="1"/>
         <v>1.4474497785262972</v>
       </c>
       <c r="J6" s="1">
-        <f>$G$2+J$16*($D$2-$D6)</f>
+        <f t="shared" si="1"/>
         <v>1.4719497785262972</v>
       </c>
       <c r="K6" s="1">
-        <f>$G$2+K$16*($D$2-$D6)</f>
+        <f t="shared" si="1"/>
         <v>1.4964497785262971</v>
       </c>
       <c r="L6" s="1">
-        <f>$G$2+L$16*($D$2-$D6)</f>
+        <f t="shared" si="1"/>
         <v>1.5209497785262971</v>
       </c>
       <c r="M6" s="1">
-        <f>$G$2+M$16*($D$2-$D6)</f>
+        <f t="shared" si="1"/>
         <v>1.5454497785262973</v>
       </c>
       <c r="N6" s="1">
-        <f>$G$2+N$16*($D$2-$D6)</f>
+        <f t="shared" si="1"/>
         <v>1.5699497785262972</v>
       </c>
       <c r="O6" s="1">
-        <f>$G$2+O$16*($D$2-$D6)</f>
+        <f t="shared" si="1"/>
         <v>1.5944497785262972</v>
       </c>
       <c r="P6" s="1">
-        <f>$G$2+P$16*($D$2-$D6)</f>
+        <f t="shared" si="1"/>
         <v>1.6189497785262972</v>
       </c>
       <c r="Q6" s="1">
-        <f>$G$2+Q$16*($D$2-$D6)</f>
+        <f t="shared" si="1"/>
         <v>1.6434497785262971</v>
       </c>
       <c r="R6" s="1">
-        <f>$G$2+R$16*($D$2-$D6)</f>
+        <f t="shared" si="1"/>
         <v>1.6679497785262973</v>
       </c>
       <c r="S6" s="1"/>
@@ -995,11 +1002,11 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7:B14" si="2">B6+5</f>
+        <f t="shared" ref="B7:B14" si="3">B6+5</f>
         <v>41.7</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.710160000000002</v>
       </c>
       <c r="D7">
@@ -1016,47 +1023,47 @@
         <v>1.4344192093203025</v>
       </c>
       <c r="H7" s="1">
-        <f>$G$2+H$16*($D$2-$D7)</f>
+        <f t="shared" si="1"/>
         <v>1.4354497785262972</v>
       </c>
       <c r="I7" s="1">
-        <f>$G$2+I$16*($D$2-$D7)</f>
+        <f t="shared" si="1"/>
         <v>1.4624497785262971</v>
       </c>
       <c r="J7" s="1">
-        <f>$G$2+J$16*($D$2-$D7)</f>
+        <f t="shared" si="1"/>
         <v>1.4894497785262972</v>
       </c>
       <c r="K7" s="1">
-        <f>$G$2+K$16*($D$2-$D7)</f>
+        <f t="shared" si="1"/>
         <v>1.5164497785262971</v>
       </c>
       <c r="L7" s="1">
-        <f>$G$2+L$16*($D$2-$D7)</f>
+        <f t="shared" si="1"/>
         <v>1.5434497785262971</v>
       </c>
       <c r="M7" s="1">
-        <f>$G$2+M$16*($D$2-$D7)</f>
+        <f t="shared" si="1"/>
         <v>1.5704497785262972</v>
       </c>
       <c r="N7" s="1">
-        <f>$G$2+N$16*($D$2-$D7)</f>
+        <f t="shared" si="1"/>
         <v>1.5974497785262971</v>
       </c>
       <c r="O7" s="1">
-        <f>$G$2+O$16*($D$2-$D7)</f>
+        <f t="shared" si="1"/>
         <v>1.6244497785262972</v>
       </c>
       <c r="P7" s="1">
-        <f>$G$2+P$16*($D$2-$D7)</f>
+        <f t="shared" si="1"/>
         <v>1.6514497785262972</v>
       </c>
       <c r="Q7" s="1">
-        <f>$G$2+Q$16*($D$2-$D7)</f>
+        <f t="shared" si="1"/>
         <v>1.6784497785262973</v>
       </c>
       <c r="R7" s="1">
-        <f>$G$2+R$16*($D$2-$D7)</f>
+        <f t="shared" si="1"/>
         <v>1.7054497785262972</v>
       </c>
       <c r="S7" s="1"/>
@@ -1084,11 +1091,11 @@
         <v>15</v>
       </c>
       <c r="B8">
+        <f t="shared" si="3"/>
+        <v>46.7</v>
+      </c>
+      <c r="C8">
         <f t="shared" si="2"/>
-        <v>46.7</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="1"/>
         <v>14.234160000000001</v>
       </c>
       <c r="D8">
@@ -1105,47 +1112,47 @@
         <v>1.4438370712466615</v>
       </c>
       <c r="H8" s="1">
-        <f>$G$2+H$16*($D$2-$D8)</f>
+        <f t="shared" si="1"/>
         <v>1.4449497785262972</v>
       </c>
       <c r="I8" s="1">
-        <f>$G$2+I$16*($D$2-$D8)</f>
+        <f t="shared" si="1"/>
         <v>1.4738497785262972</v>
       </c>
       <c r="J8" s="1">
-        <f>$G$2+J$16*($D$2-$D8)</f>
+        <f t="shared" si="1"/>
         <v>1.5027497785262971</v>
       </c>
       <c r="K8" s="1">
-        <f>$G$2+K$16*($D$2-$D8)</f>
+        <f t="shared" si="1"/>
         <v>1.5316497785262972</v>
       </c>
       <c r="L8" s="1">
-        <f>$G$2+L$16*($D$2-$D8)</f>
+        <f t="shared" si="1"/>
         <v>1.5605497785262972</v>
       </c>
       <c r="M8" s="1">
-        <f>$G$2+M$16*($D$2-$D8)</f>
+        <f t="shared" si="1"/>
         <v>1.5894497785262971</v>
       </c>
       <c r="N8" s="1">
-        <f>$G$2+N$16*($D$2-$D8)</f>
+        <f t="shared" si="1"/>
         <v>1.6183497785262972</v>
       </c>
       <c r="O8" s="1">
-        <f>$G$2+O$16*($D$2-$D8)</f>
+        <f t="shared" si="1"/>
         <v>1.6472497785262972</v>
       </c>
       <c r="P8" s="1">
-        <f>$G$2+P$16*($D$2-$D8)</f>
+        <f t="shared" si="1"/>
         <v>1.6761497785262973</v>
       </c>
       <c r="Q8" s="1">
-        <f>$G$2+Q$16*($D$2-$D8)</f>
+        <f t="shared" si="1"/>
         <v>1.7050497785262972</v>
       </c>
       <c r="R8" s="1">
-        <f>$G$2+R$16*($D$2-$D8)</f>
+        <f t="shared" si="1"/>
         <v>1.7339497785262972</v>
       </c>
       <c r="S8" s="1"/>
@@ -1173,11 +1180,11 @@
         <v>16</v>
       </c>
       <c r="B9">
+        <f t="shared" si="3"/>
+        <v>51.7</v>
+      </c>
+      <c r="C9">
         <f t="shared" si="2"/>
-        <v>51.7</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="1"/>
         <v>15.758160000000002</v>
       </c>
       <c r="D9">
@@ -1194,47 +1201,47 @@
         <v>1.4509404753785293</v>
       </c>
       <c r="H9" s="1">
-        <f>$G$2+H$16*($D$2-$D9)</f>
+        <f t="shared" si="1"/>
         <v>1.4524497785262973</v>
       </c>
       <c r="I9" s="1">
-        <f>$G$2+I$16*($D$2-$D9)</f>
+        <f t="shared" si="1"/>
         <v>1.4828497785262973</v>
       </c>
       <c r="J9" s="1">
-        <f>$G$2+J$16*($D$2-$D9)</f>
+        <f t="shared" si="1"/>
         <v>1.5132497785262973</v>
       </c>
       <c r="K9" s="1">
-        <f>$G$2+K$16*($D$2-$D9)</f>
+        <f t="shared" si="1"/>
         <v>1.5436497785262973</v>
       </c>
       <c r="L9" s="1">
-        <f>$G$2+L$16*($D$2-$D9)</f>
+        <f t="shared" si="1"/>
         <v>1.5740497785262972</v>
       </c>
       <c r="M9" s="1">
-        <f>$G$2+M$16*($D$2-$D9)</f>
+        <f t="shared" si="1"/>
         <v>1.6044497785262972</v>
       </c>
       <c r="N9" s="1">
-        <f>$G$2+N$16*($D$2-$D9)</f>
+        <f t="shared" si="1"/>
         <v>1.6348497785262972</v>
       </c>
       <c r="O9" s="1">
-        <f>$G$2+O$16*($D$2-$D9)</f>
+        <f t="shared" si="1"/>
         <v>1.6652497785262972</v>
       </c>
       <c r="P9" s="1">
-        <f>$G$2+P$16*($D$2-$D9)</f>
+        <f t="shared" si="1"/>
         <v>1.6956497785262972</v>
       </c>
       <c r="Q9" s="1">
-        <f>$G$2+Q$16*($D$2-$D9)</f>
+        <f t="shared" si="1"/>
         <v>1.7260497785262974</v>
       </c>
       <c r="R9" s="1">
-        <f>$G$2+R$16*($D$2-$D9)</f>
+        <f t="shared" si="1"/>
         <v>1.7564497785262974</v>
       </c>
       <c r="S9" s="1"/>
@@ -1262,11 +1269,11 @@
         <v>17</v>
       </c>
       <c r="B10">
+        <f t="shared" si="3"/>
+        <v>56.7</v>
+      </c>
+      <c r="C10">
         <f t="shared" si="2"/>
-        <v>56.7</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="1"/>
         <v>17.282160000000001</v>
       </c>
       <c r="D10">
@@ -1283,47 +1290,47 @@
         <v>1.4581697270114942</v>
       </c>
       <c r="H10" s="1">
-        <f>$G$2+H$16*($D$2-$D10)</f>
+        <f t="shared" si="1"/>
         <v>1.4589497785262973</v>
       </c>
       <c r="I10" s="1">
-        <f>$G$2+I$16*($D$2-$D10)</f>
+        <f t="shared" si="1"/>
         <v>1.4906497785262971</v>
       </c>
       <c r="J10" s="1">
-        <f>$G$2+J$16*($D$2-$D10)</f>
+        <f t="shared" si="1"/>
         <v>1.5223497785262972</v>
       </c>
       <c r="K10" s="1">
-        <f>$G$2+K$16*($D$2-$D10)</f>
+        <f t="shared" si="1"/>
         <v>1.5540497785262972</v>
       </c>
       <c r="L10" s="1">
-        <f>$G$2+L$16*($D$2-$D10)</f>
+        <f t="shared" si="1"/>
         <v>1.5857497785262971</v>
       </c>
       <c r="M10" s="1">
-        <f>$G$2+M$16*($D$2-$D10)</f>
+        <f t="shared" si="1"/>
         <v>1.6174497785262971</v>
       </c>
       <c r="N10" s="1">
-        <f>$G$2+N$16*($D$2-$D10)</f>
+        <f t="shared" si="1"/>
         <v>1.6491497785262972</v>
       </c>
       <c r="O10" s="1">
-        <f>$G$2+O$16*($D$2-$D10)</f>
+        <f t="shared" si="1"/>
         <v>1.6808497785262972</v>
       </c>
       <c r="P10" s="1">
-        <f>$G$2+P$16*($D$2-$D10)</f>
+        <f t="shared" si="1"/>
         <v>1.7125497785262973</v>
       </c>
       <c r="Q10" s="1">
-        <f>$G$2+Q$16*($D$2-$D10)</f>
+        <f t="shared" si="1"/>
         <v>1.7442497785262971</v>
       </c>
       <c r="R10" s="1">
-        <f>$G$2+R$16*($D$2-$D10)</f>
+        <f t="shared" si="1"/>
         <v>1.7759497785262972</v>
       </c>
       <c r="S10" s="1"/>
@@ -1351,11 +1358,11 @@
         <v>18</v>
       </c>
       <c r="B11">
+        <f t="shared" si="3"/>
+        <v>61.7</v>
+      </c>
+      <c r="C11">
         <f t="shared" si="2"/>
-        <v>61.7</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="1"/>
         <v>18.806160000000002</v>
       </c>
       <c r="D11">
@@ -1372,47 +1379,47 @@
         <v>1.4643493200265034</v>
       </c>
       <c r="H11" s="1">
-        <f>$G$2+H$16*($D$2-$D11)</f>
+        <f t="shared" si="1"/>
         <v>1.4644497785262971</v>
       </c>
       <c r="I11" s="1">
-        <f>$G$2+I$16*($D$2-$D11)</f>
+        <f t="shared" si="1"/>
         <v>1.4972497785262973</v>
       </c>
       <c r="J11" s="1">
-        <f>$G$2+J$16*($D$2-$D11)</f>
+        <f t="shared" si="1"/>
         <v>1.5300497785262972</v>
       </c>
       <c r="K11" s="1">
-        <f>$G$2+K$16*($D$2-$D11)</f>
+        <f t="shared" si="1"/>
         <v>1.5628497785262971</v>
       </c>
       <c r="L11" s="1">
-        <f>$G$2+L$16*($D$2-$D11)</f>
+        <f t="shared" si="1"/>
         <v>1.5956497785262971</v>
       </c>
       <c r="M11" s="1">
-        <f>$G$2+M$16*($D$2-$D11)</f>
+        <f t="shared" si="1"/>
         <v>1.628449778526297</v>
       </c>
       <c r="N11" s="1">
-        <f>$G$2+N$16*($D$2-$D11)</f>
+        <f t="shared" si="1"/>
         <v>1.6612497785262972</v>
       </c>
       <c r="O11" s="1">
-        <f>$G$2+O$16*($D$2-$D11)</f>
+        <f t="shared" si="1"/>
         <v>1.6940497785262971</v>
       </c>
       <c r="P11" s="1">
-        <f>$G$2+P$16*($D$2-$D11)</f>
+        <f t="shared" si="1"/>
         <v>1.7268497785262973</v>
       </c>
       <c r="Q11" s="1">
-        <f>$G$2+Q$16*($D$2-$D11)</f>
+        <f t="shared" si="1"/>
         <v>1.7596497785262972</v>
       </c>
       <c r="R11" s="1">
-        <f>$G$2+R$16*($D$2-$D11)</f>
+        <f t="shared" si="1"/>
         <v>1.7924497785262972</v>
       </c>
       <c r="S11" s="1"/>
@@ -1440,11 +1447,11 @@
         <v>19</v>
       </c>
       <c r="B12">
+        <f t="shared" si="3"/>
+        <v>66.7</v>
+      </c>
+      <c r="C12">
         <f t="shared" si="2"/>
-        <v>66.7</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="1"/>
         <v>20.330160000000003</v>
       </c>
       <c r="D12">
@@ -1461,47 +1468,47 @@
         <v>1.4684428549768105</v>
       </c>
       <c r="H12" s="1">
-        <f>$G$2+H$16*($D$2-$D12)</f>
+        <f t="shared" si="1"/>
         <v>1.4689497785262973</v>
       </c>
       <c r="I12" s="1">
-        <f>$G$2+I$16*($D$2-$D12)</f>
+        <f t="shared" si="1"/>
         <v>1.5026497785262971</v>
       </c>
       <c r="J12" s="1">
-        <f>$G$2+J$16*($D$2-$D12)</f>
+        <f t="shared" si="1"/>
         <v>1.5363497785262972</v>
       </c>
       <c r="K12" s="1">
-        <f>$G$2+K$16*($D$2-$D12)</f>
+        <f t="shared" si="1"/>
         <v>1.5700497785262972</v>
       </c>
       <c r="L12" s="1">
-        <f>$G$2+L$16*($D$2-$D12)</f>
+        <f t="shared" si="1"/>
         <v>1.6037497785262973</v>
       </c>
       <c r="M12" s="1">
-        <f>$G$2+M$16*($D$2-$D12)</f>
+        <f t="shared" si="1"/>
         <v>1.6374497785262971</v>
       </c>
       <c r="N12" s="1">
-        <f>$G$2+N$16*($D$2-$D12)</f>
+        <f t="shared" si="1"/>
         <v>1.6711497785262972</v>
       </c>
       <c r="O12" s="1">
-        <f>$G$2+O$16*($D$2-$D12)</f>
+        <f t="shared" si="1"/>
         <v>1.7048497785262973</v>
       </c>
       <c r="P12" s="1">
-        <f>$G$2+P$16*($D$2-$D12)</f>
+        <f t="shared" si="1"/>
         <v>1.7385497785262971</v>
       </c>
       <c r="Q12" s="1">
-        <f>$G$2+Q$16*($D$2-$D12)</f>
+        <f t="shared" si="1"/>
         <v>1.7722497785262972</v>
       </c>
       <c r="R12" s="1">
-        <f>$G$2+R$16*($D$2-$D12)</f>
+        <f t="shared" si="1"/>
         <v>1.8059497785262972</v>
       </c>
       <c r="S12" s="1"/>
@@ -1529,11 +1536,11 @@
         <v>20</v>
       </c>
       <c r="B13">
+        <f t="shared" si="3"/>
+        <v>71.7</v>
+      </c>
+      <c r="C13">
         <f t="shared" si="2"/>
-        <v>71.7</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="1"/>
         <v>21.85416</v>
       </c>
       <c r="D13">
@@ -1550,47 +1557,47 @@
         <v>1.4726547347569812</v>
       </c>
       <c r="H13" s="1">
-        <f>$G$2+H$16*($D$2-$D13)</f>
+        <f t="shared" si="1"/>
         <v>1.4729497785262973</v>
       </c>
       <c r="I13" s="1">
-        <f>$G$2+I$16*($D$2-$D13)</f>
+        <f t="shared" si="1"/>
         <v>1.5074497785262972</v>
       </c>
       <c r="J13" s="1">
-        <f>$G$2+J$16*($D$2-$D13)</f>
+        <f t="shared" si="1"/>
         <v>1.5419497785262972</v>
       </c>
       <c r="K13" s="1">
-        <f>$G$2+K$16*($D$2-$D13)</f>
+        <f t="shared" si="1"/>
         <v>1.5764497785262972</v>
       </c>
       <c r="L13" s="1">
-        <f>$G$2+L$16*($D$2-$D13)</f>
+        <f t="shared" si="1"/>
         <v>1.6109497785262972</v>
       </c>
       <c r="M13" s="1">
-        <f>$G$2+M$16*($D$2-$D13)</f>
+        <f t="shared" si="1"/>
         <v>1.6454497785262971</v>
       </c>
       <c r="N13" s="1">
-        <f>$G$2+N$16*($D$2-$D13)</f>
+        <f t="shared" si="1"/>
         <v>1.6799497785262971</v>
       </c>
       <c r="O13" s="1">
-        <f>$G$2+O$16*($D$2-$D13)</f>
+        <f t="shared" si="1"/>
         <v>1.7144497785262973</v>
       </c>
       <c r="P13" s="1">
-        <f>$G$2+P$16*($D$2-$D13)</f>
+        <f t="shared" si="1"/>
         <v>1.7489497785262973</v>
       </c>
       <c r="Q13" s="1">
-        <f>$G$2+Q$16*($D$2-$D13)</f>
+        <f t="shared" si="1"/>
         <v>1.7834497785262973</v>
       </c>
       <c r="R13" s="1">
-        <f>$G$2+R$16*($D$2-$D13)</f>
+        <f t="shared" si="1"/>
         <v>1.8179497785262972</v>
       </c>
       <c r="S13" s="1"/>
@@ -1618,11 +1625,11 @@
         <v>21</v>
       </c>
       <c r="B14">
+        <f t="shared" si="3"/>
+        <v>76.7</v>
+      </c>
+      <c r="C14">
         <f t="shared" si="2"/>
-        <v>76.7</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="1"/>
         <v>23.378160000000001</v>
       </c>
       <c r="D14">
@@ -1639,51 +1646,54 @@
         <v>1.479929519132392</v>
       </c>
       <c r="H14" s="1">
-        <f>$G$2+H$16*($D$2-$D14)</f>
+        <f t="shared" si="1"/>
         <v>1.4760997785262973</v>
       </c>
       <c r="I14" s="1">
-        <f>$G$2+I$16*($D$2-$D14)</f>
+        <f t="shared" si="1"/>
         <v>1.5112297785262971</v>
       </c>
       <c r="J14" s="1">
-        <f>$G$2+J$16*($D$2-$D14)</f>
+        <f t="shared" si="1"/>
         <v>1.5463597785262972</v>
       </c>
       <c r="K14" s="1">
-        <f>$G$2+K$16*($D$2-$D14)</f>
+        <f t="shared" si="1"/>
         <v>1.5814897785262971</v>
       </c>
       <c r="L14" s="1">
-        <f>$G$2+L$16*($D$2-$D14)</f>
+        <f t="shared" si="1"/>
         <v>1.6166197785262972</v>
       </c>
       <c r="M14" s="1">
-        <f>$G$2+M$16*($D$2-$D14)</f>
+        <f t="shared" si="1"/>
         <v>1.6517497785262971</v>
       </c>
       <c r="N14" s="1">
-        <f>$G$2+N$16*($D$2-$D14)</f>
+        <f t="shared" si="1"/>
         <v>1.686879778526297</v>
       </c>
       <c r="O14" s="1">
-        <f>$G$2+O$16*($D$2-$D14)</f>
+        <f t="shared" si="1"/>
         <v>1.7220097785262971</v>
       </c>
       <c r="P14" s="1">
-        <f>$G$2+P$16*($D$2-$D14)</f>
+        <f t="shared" si="1"/>
         <v>1.7571397785262972</v>
       </c>
       <c r="Q14" s="1">
-        <f>$G$2+Q$16*($D$2-$D14)</f>
+        <f t="shared" si="1"/>
         <v>1.7922697785262973</v>
       </c>
       <c r="R14" s="1">
-        <f>$G$2+R$16*($D$2-$D14)</f>
+        <f t="shared" si="1"/>
         <v>1.8273997785262972</v>
       </c>
       <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
+      <c r="T14" s="4">
+        <f>0.13/G14</f>
+        <v>8.7842021068822551E-2</v>
+      </c>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
@@ -1715,39 +1725,39 @@
         <v>0.6</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" ref="J16:R16" si="3">I16+$G$17</f>
+        <f t="shared" ref="J16:R16" si="4">I16+$G$17</f>
         <v>0.7</v>
       </c>
       <c r="K16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.79999999999999993</v>
       </c>
       <c r="L16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="M16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.0999999999999999</v>
       </c>
       <c r="O16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.2</v>
       </c>
       <c r="P16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3</v>
       </c>
       <c r="Q16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.4000000000000001</v>
       </c>
       <c r="R16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.5000000000000002</v>
       </c>
       <c r="S16" s="1"/>
@@ -1781,4 +1791,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{95965d95-ecc0-4720-b759-1f33c42ed7da}" enabled="1" method="Standard" siteId="{a0f29d7e-28cd-4f54-8442-7885aee7c080}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>